<commit_message>
Add function to rfd po and jo
</commit_message>
<xml_diff>
--- a/storage/app/imports/PurchaseRequestFormcenpribcd.xlsx
+++ b/storage/app/imports/PurchaseRequestFormcenpribcd.xlsx
@@ -893,7 +893,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:K9"/>
+      <selection activeCell="I10" sqref="I10:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,9 +1057,7 @@
       <c r="H10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="27">
-        <v>1</v>
-      </c>
+      <c r="I10" s="27"/>
       <c r="J10" s="28"/>
       <c r="K10" s="29"/>
     </row>
@@ -1143,9 +1141,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
-      <c r="I14" s="10">
-        <v>1</v>
-      </c>
+      <c r="I14" s="10"/>
       <c r="J14" s="17">
         <v>45608</v>
       </c>
@@ -1170,9 +1166,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="10">
-        <v>2</v>
-      </c>
+      <c r="I15" s="10"/>
       <c r="J15" s="17">
         <v>45609</v>
       </c>
@@ -1197,9 +1191,7 @@
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="10">
-        <v>3</v>
-      </c>
+      <c r="I16" s="10"/>
       <c r="J16" s="17">
         <v>45610</v>
       </c>
@@ -1224,9 +1216,7 @@
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
-      <c r="I17" s="10">
-        <v>4</v>
-      </c>
+      <c r="I17" s="10"/>
       <c r="J17" s="17">
         <v>45611</v>
       </c>
@@ -1251,9 +1241,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
-      <c r="I18" s="10">
-        <v>5</v>
-      </c>
+      <c r="I18" s="10"/>
       <c r="J18" s="17">
         <v>45612</v>
       </c>

</xml_diff>

<commit_message>
Fix uom and offer not displaying in joi
</commit_message>
<xml_diff>
--- a/storage/app/imports/PurchaseRequestFormcenpribcd.xlsx
+++ b/storage/app/imports/PurchaseRequestFormcenpribcd.xlsx
@@ -258,13 +258,13 @@
     <t>Item5</t>
   </si>
   <si>
-    <t xml:space="preserve"> department11</t>
-  </si>
-  <si>
     <t>Jonah Faye Benares</t>
   </si>
   <si>
-    <t>PR10011234</t>
+    <t>PR100112341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  IT-Bacolod</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I7" sqref="I7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1005,7 @@
         <v>17</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J7" s="24"/>
       <c r="K7" s="25"/>
@@ -1024,7 +1024,7 @@
         <v>62</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="25"/>
@@ -1043,7 +1043,7 @@
         <v>5</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="25"/>
@@ -1057,7 +1057,9 @@
       <c r="H10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="23"/>
+      <c r="I10" s="23">
+        <v>0</v>
+      </c>
       <c r="J10" s="24"/>
       <c r="K10" s="25"/>
     </row>

</xml_diff>